<commit_message>
New code changes for the bypaas bot detection and remove retry
</commit_message>
<xml_diff>
--- a/testData/test.xlsx
+++ b/testData/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{373587A9-74F6-47E0-B60C-DEC30BFDD8B3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9C72C550-04B6-4F8F-9D93-5D905DA20D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EF4DF7-3A4D-45C7-A3FB-00D4BA47F938}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>action</t>
   </si>
@@ -56,9 +56,6 @@
     <t>goto</t>
   </si>
   <si>
-    <t>scroll</t>
-  </si>
-  <si>
     <t>TestID</t>
   </si>
   <si>
@@ -74,74 +71,35 @@
     <t>locatorType</t>
   </si>
   <si>
-    <t>button</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>h2</t>
-  </si>
-  <si>
-    <t>https://selectorshub.com/xpath-practice-page/</t>
-  </si>
-  <si>
-    <t>Bottom Modal</t>
-  </si>
-  <si>
-    <t>Open Modal</t>
-  </si>
-  <si>
-    <t>Subscribe to our youtube channel</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>vab@email.com</t>
-  </si>
-  <si>
     <t>waitfortext</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>h4</t>
+    <t>https://www.scrapingcourse.com/ecommerce/</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
   <si>
     <t>assert</t>
   </si>
   <si>
-    <t>cartassert</t>
-  </si>
-  <si>
-    <t>Model Alert Popup</t>
-  </si>
-  <si>
-    <t>div[data-widget_type="text-editor.default"] p</t>
-  </si>
-  <si>
-    <t>Innovation Inspired Automation!!</t>
-  </si>
-  <si>
-    <t>#firstNameParser,nameNode</t>
-  </si>
-  <si>
-    <t>#lastNameParser,nameNode</t>
+    <t>div a[rel="home"]</t>
+  </si>
+  <si>
+    <t>Ecommerce Test Site</t>
+  </si>
+  <si>
+    <t>Ecommerce Test Site to Learn Web Scraping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecommerce Test Site </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +118,12 @@
     <font>
       <sz val="8"/>
       <color rgb="FFCCCCCC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292F"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -185,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -194,6 +158,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,7 +442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -492,10 +459,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -504,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -518,42 +485,41 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2"/>
       <c r="G2" s="1">
         <v>1000</v>
       </c>
       <c r="H2" s="1">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="1">
         <v>1000</v>
       </c>
@@ -561,194 +527,27 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="G4" s="1">
         <v>1000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -768,10 +567,7 @@
       <c r="F33" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{FBD3D60D-B9CD-4363-B97A-69A7DD7957F6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code for bot bypass
</commit_message>
<xml_diff>
--- a/testData/test.xlsx
+++ b/testData/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{373587A9-74F6-47E0-B60C-DEC30BFDD8B3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9C72C550-04B6-4F8F-9D93-5D905DA20D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EF4DF7-3A4D-45C7-A3FB-00D4BA47F938}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>action</t>
   </si>
@@ -56,9 +56,6 @@
     <t>goto</t>
   </si>
   <si>
-    <t>scroll</t>
-  </si>
-  <si>
     <t>TestID</t>
   </si>
   <si>
@@ -74,74 +71,35 @@
     <t>locatorType</t>
   </si>
   <si>
-    <t>button</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>h2</t>
-  </si>
-  <si>
-    <t>https://selectorshub.com/xpath-practice-page/</t>
-  </si>
-  <si>
-    <t>Bottom Modal</t>
-  </si>
-  <si>
-    <t>Open Modal</t>
-  </si>
-  <si>
-    <t>Subscribe to our youtube channel</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>vab@email.com</t>
-  </si>
-  <si>
     <t>waitfortext</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>h4</t>
+    <t>https://www.scrapingcourse.com/ecommerce/</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
   <si>
     <t>assert</t>
   </si>
   <si>
-    <t>cartassert</t>
-  </si>
-  <si>
-    <t>Model Alert Popup</t>
-  </si>
-  <si>
-    <t>div[data-widget_type="text-editor.default"] p</t>
-  </si>
-  <si>
-    <t>Innovation Inspired Automation!!</t>
-  </si>
-  <si>
-    <t>#firstNameParser,nameNode</t>
-  </si>
-  <si>
-    <t>#lastNameParser,nameNode</t>
+    <t>div a[rel="home"]</t>
+  </si>
+  <si>
+    <t>Ecommerce Test Site</t>
+  </si>
+  <si>
+    <t>Ecommerce Test Site to Learn Web Scraping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecommerce Test Site </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +118,12 @@
     <font>
       <sz val="8"/>
       <color rgb="FFCCCCCC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292F"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -185,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -194,6 +158,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,7 +442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -492,10 +459,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -504,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -518,42 +485,41 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2"/>
       <c r="G2" s="1">
         <v>1000</v>
       </c>
       <c r="H2" s="1">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="1">
         <v>1000</v>
       </c>
@@ -561,194 +527,27 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="G4" s="1">
         <v>1000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -768,10 +567,7 @@
       <c r="F33" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{FBD3D60D-B9CD-4363-B97A-69A7DD7957F6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new changes for bot detection
</commit_message>
<xml_diff>
--- a/testData/test.xlsx
+++ b/testData/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9C72C550-04B6-4F8F-9D93-5D905DA20D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EF4DF7-3A4D-45C7-A3FB-00D4BA47F938}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{9C72C550-04B6-4F8F-9D93-5D905DA20D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EB4620D-79AF-4C70-915B-ECA72DF77198}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>action</t>
   </si>
@@ -74,25 +74,16 @@
     <t>waitfortext</t>
   </si>
   <si>
-    <t>https://www.scrapingcourse.com/ecommerce/</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>assert</t>
-  </si>
-  <si>
-    <t>div a[rel="home"]</t>
-  </si>
-  <si>
-    <t>Ecommerce Test Site</t>
-  </si>
-  <si>
-    <t>Ecommerce Test Site to Learn Web Scraping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecommerce Test Site </t>
+    <t>Mattresses</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>https://www.nectarsleep.com</t>
   </si>
 </sst>
 </file>
@@ -442,9 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -494,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
       <c r="G2" s="1">
@@ -515,10 +504,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
         <v>1000</v>
@@ -538,16 +527,17 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="1">
         <v>1000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -567,7 +557,10 @@
       <c r="F33" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4D77B558-21AC-458F-B75B-ECC509ED4B88}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new changes for bot bypass
</commit_message>
<xml_diff>
--- a/testData/test.xlsx
+++ b/testData/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9C72C550-04B6-4F8F-9D93-5D905DA20D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EF4DF7-3A4D-45C7-A3FB-00D4BA47F938}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{9C72C550-04B6-4F8F-9D93-5D905DA20D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EB4620D-79AF-4C70-915B-ECA72DF77198}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>action</t>
   </si>
@@ -74,25 +74,16 @@
     <t>waitfortext</t>
   </si>
   <si>
-    <t>https://www.scrapingcourse.com/ecommerce/</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>assert</t>
-  </si>
-  <si>
-    <t>div a[rel="home"]</t>
-  </si>
-  <si>
-    <t>Ecommerce Test Site</t>
-  </si>
-  <si>
-    <t>Ecommerce Test Site to Learn Web Scraping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecommerce Test Site </t>
+    <t>Mattresses</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>https://www.nectarsleep.com</t>
   </si>
 </sst>
 </file>
@@ -442,9 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -494,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
       <c r="G2" s="1">
@@ -515,10 +504,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
         <v>1000</v>
@@ -538,16 +527,17 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="1">
         <v>1000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -567,7 +557,10 @@
       <c r="F33" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4D77B558-21AC-458F-B75B-ECC509ED4B88}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>